<commit_message>
test recap groupe 4 v2
</commit_message>
<xml_diff>
--- a/Tests/Groupe_4/test_recap_group_4.xlsx
+++ b/Tests/Groupe_4/test_recap_group_4.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>nom fichier</t>
   </si>
@@ -73,6 +73,15 @@
   <si>
     <t>le fichier en entier
 (car pas de fonction)</t>
+  </si>
+  <si>
+    <t>une erreur est levée</t>
+  </si>
+  <si>
+    <t>cas nominal (aucune erreur n'est levée)</t>
+  </si>
+  <si>
+    <t>le temps d'exécution du message s'affiche</t>
   </si>
 </sst>
 </file>
@@ -441,7 +450,7 @@
   <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -558,16 +567,25 @@
       <c r="C8" s="10">
         <v>43115</v>
       </c>
+      <c r="D8" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="10"/>
+      <c r="D9" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
       <c r="B10" s="6"/>
       <c r="C10" s="10"/>
+      <c r="D10" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>

</xml_diff>